<commit_message>
commit prior to adding legend
</commit_message>
<xml_diff>
--- a/data/mn_data_pull.xlsx
+++ b/data/mn_data_pull.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="700" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="-38400" yWindow="1220" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="county_decile" sheetId="1" r:id="rId1"/>
@@ -363,7 +363,7 @@
   <dimension ref="A1:D397"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5936,7 +5936,7 @@
   <dimension ref="A1:D109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>